<commit_message>
i285--unzip flow bug fix
</commit_message>
<xml_diff>
--- a/tmp_client/doc/TMP_example/diamond_regression.xlsx
+++ b/tmp_client/doc/TMP_example/diamond_regression.xlsx
@@ -26,9 +26,9 @@
   </definedNames>
   <calcPr calcId="144525"/>
   <customWorkbookViews>
+    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
+    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
     <customWorkbookView name="Jason Wang - Personal View" guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="2"/>
-    <customWorkbookView name="Xueying Li - Personal View" guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" personalView="1" yWindow="337" windowWidth="1878" windowHeight="703" activeSheetId="1"/>
-    <customWorkbookView name="Cherry Xu - Personal View" guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" personalView="1" maximized="1" windowWidth="1916" windowHeight="835" activeSheetId="2"/>
   </customWorkbookViews>
 </workbook>
 </file>
@@ -597,9 +597,6 @@
     <t>no</t>
   </si>
   <si>
-    <t>no,7z,zip,gzip,bzip2,tar</t>
-  </si>
-  <si>
     <t>script_url</t>
   </si>
   <si>
@@ -994,6 +991,9 @@
   </si>
   <si>
     <t>user prefer launch path setting</t>
+  </si>
+  <si>
+    <t>no,sevenz,bz2,bzip2,tbz2,tbz,gz,gzip,tgz,tar,zip,targz,tarbz,tarbz2</t>
   </si>
 </sst>
 </file>
@@ -1567,7 +1567,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5">
       <alignment vertical="center"/>
@@ -1785,6 +1785,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="5" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="33" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1797,107 +1800,107 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="35" xfId="4" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Check Cell" xfId="4" builtinId="23"/>
@@ -4355,46 +4358,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{C3911F6D-7671-4AF3-8B15-3A104438C863}" diskRevisions="1" revisionId="1" version="2">
-  <header guid="{D6C683F4-DECC-4CC2-9E87-3C85EDCCE6F3}" dateTime="2020-07-10T18:35:27" maxSheetId="5" userName="Jason Wang" r:id="rId1">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{C3911F6D-7671-4AF3-8B15-3A104438C863}" dateTime="2020-07-10T18:35:37" maxSheetId="5" userName="Jason Wang" r:id="rId2">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-</headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_E811CF45_D5B3_4449_84AE_1514F9E9258F_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>case!$A$2:$AD$46</formula>
-    <oldFormula>case!$A$2:$AD$46</oldFormula>
-  </rdn>
-  <rcv guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4687,7 +4650,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -4770,7 +4733,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="BrxOpSv5Qn+u2wRjM+utC6UYLrvUI+Gay+w6zPQp8zz+/5I1udizjqbZ6brqgp9h1Ud3zJVEOn/q/bgrm9i81A==" saltValue="wt9VphKaQ5GnARCLMZGRjA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="B35" sqref="B35"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -4779,8 +4743,7 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="B35" sqref="B35"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
     </customSheetView>
@@ -4831,40 +4794,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="60" customFormat="1">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="76" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="76"/>
-      <c r="Y1" s="76"/>
-      <c r="Z1" s="76"/>
-      <c r="AA1" s="76"/>
-      <c r="AB1" s="76"/>
-      <c r="AC1" s="76"/>
-      <c r="AD1" s="76"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
     </row>
     <row r="2" spans="1:30" s="60" customFormat="1">
       <c r="A2" s="63" t="s">
@@ -6382,12 +6345,12 @@
   <sheetProtection algorithmName="SHA-512" hashValue="4C55417S7/WEfM6p9p+2qxLa3pFuuwTQvkVS+xLflxPJ6JUMhmXb8UBi2EhWPKsWHpV7wPPZoM4Ci73L5pzjfA==" saltValue="OVPlytvnGy6tQU/SUgOtyg==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A2:AD46"/>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="M38" sqref="M38"/>
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
+      <selection activeCell="C23" sqref="C23"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:AD46"/>
+      <autoFilter ref="A2:Y2"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}" scale="85" showAutoFilter="1">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
@@ -6396,12 +6359,12 @@
       <pageSetup paperSize="9" orientation="portrait"/>
       <autoFilter ref="A2:Y2"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}" scale="85" showAutoFilter="1">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" state="frozen"/>
-      <selection activeCell="C23" sqref="C23"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="85" showAutoFilter="1">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="M38" sqref="M38"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait"/>
-      <autoFilter ref="A2:Y2"/>
+      <autoFilter ref="A2:AD46"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -6479,8 +6442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N238"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F172" sqref="F172"/>
+    <sheetView topLeftCell="A193" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C209" sqref="C209:E209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -6541,17 +6504,17 @@
       <c r="E111" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="F111" s="106" t="s">
+      <c r="F111" s="78" t="s">
         <v>144</v>
       </c>
-      <c r="G111" s="107"/>
-      <c r="H111" s="107"/>
-      <c r="I111" s="107"/>
-      <c r="J111" s="107"/>
-      <c r="K111" s="107"/>
-      <c r="L111" s="107"/>
-      <c r="M111" s="107"/>
-      <c r="N111" s="108"/>
+      <c r="G111" s="79"/>
+      <c r="H111" s="79"/>
+      <c r="I111" s="79"/>
+      <c r="J111" s="79"/>
+      <c r="K111" s="79"/>
+      <c r="L111" s="79"/>
+      <c r="M111" s="79"/>
+      <c r="N111" s="80"/>
     </row>
     <row r="112" spans="1:14">
       <c r="A112" s="6" t="s">
@@ -7415,7 +7378,7 @@
       <c r="A147" s="19">
         <v>1</v>
       </c>
-      <c r="B147" s="77" t="s">
+      <c r="B147" s="108" t="s">
         <v>5</v>
       </c>
       <c r="C147" s="65" t="s">
@@ -7441,7 +7404,7 @@
       <c r="A148" s="19">
         <v>2</v>
       </c>
-      <c r="B148" s="78"/>
+      <c r="B148" s="109"/>
       <c r="C148" s="21" t="s">
         <v>177</v>
       </c>
@@ -7463,7 +7426,7 @@
       <c r="A149" s="19">
         <v>3</v>
       </c>
-      <c r="B149" s="78"/>
+      <c r="B149" s="109"/>
       <c r="C149" s="21" t="s">
         <v>22</v>
       </c>
@@ -7481,7 +7444,7 @@
       <c r="A150" s="19">
         <v>4</v>
       </c>
-      <c r="B150" s="78"/>
+      <c r="B150" s="109"/>
       <c r="C150" s="21" t="s">
         <v>179</v>
       </c>
@@ -7503,7 +7466,7 @@
       <c r="A151" s="19">
         <v>5</v>
       </c>
-      <c r="B151" s="78"/>
+      <c r="B151" s="109"/>
       <c r="C151" s="65" t="s">
         <v>181</v>
       </c>
@@ -7527,7 +7490,7 @@
       <c r="A152" s="19">
         <v>6</v>
       </c>
-      <c r="B152" s="78"/>
+      <c r="B152" s="109"/>
       <c r="C152" s="65" t="s">
         <v>185</v>
       </c>
@@ -7540,8 +7503,8 @@
       <c r="F152" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="G152" s="21" t="s">
-        <v>187</v>
+      <c r="G152" s="73" t="s">
+        <v>317</v>
       </c>
       <c r="H152" s="11" t="s">
         <v>184</v>
@@ -7551,9 +7514,9 @@
       <c r="A153" s="19">
         <v>7</v>
       </c>
-      <c r="B153" s="78"/>
+      <c r="B153" s="109"/>
       <c r="C153" s="21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D153" s="21" t="s">
         <v>173</v>
@@ -7571,9 +7534,9 @@
       <c r="A154" s="19">
         <v>8</v>
       </c>
-      <c r="B154" s="78"/>
+      <c r="B154" s="109"/>
       <c r="C154" s="65" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D154" s="21" t="s">
         <v>173</v>
@@ -7593,9 +7556,9 @@
       <c r="A155" s="19">
         <v>9</v>
       </c>
-      <c r="B155" s="78"/>
+      <c r="B155" s="109"/>
       <c r="C155" s="65" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D155" s="21" t="s">
         <v>173</v>
@@ -7617,9 +7580,9 @@
       <c r="A156" s="19">
         <v>10</v>
       </c>
-      <c r="B156" s="78"/>
+      <c r="B156" s="109"/>
       <c r="C156" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D156" s="21" t="s">
         <v>173</v>
@@ -7630,8 +7593,8 @@
       <c r="F156" s="21" t="s">
         <v>186</v>
       </c>
-      <c r="G156" s="21" t="s">
-        <v>187</v>
+      <c r="G156" s="73" t="s">
+        <v>317</v>
       </c>
       <c r="H156" s="11" t="s">
         <v>184</v>
@@ -7641,9 +7604,9 @@
       <c r="A157" s="19">
         <v>11</v>
       </c>
-      <c r="B157" s="78"/>
+      <c r="B157" s="109"/>
       <c r="C157" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D157" s="21" t="s">
         <v>173</v>
@@ -7656,38 +7619,38 @@
         <v>175</v>
       </c>
       <c r="H157" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="158" spans="1:8">
       <c r="A158" s="19">
         <v>12</v>
       </c>
-      <c r="B158" s="78"/>
+      <c r="B158" s="109"/>
       <c r="C158" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D158" s="21" t="s">
         <v>173</v>
       </c>
       <c r="E158" s="21"/>
       <c r="F158" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="G158" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="G158" s="21" t="s">
+      <c r="H158" s="11" t="s">
         <v>196</v>
-      </c>
-      <c r="H158" s="11" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="159" spans="1:8">
       <c r="A159" s="19">
         <v>13</v>
       </c>
-      <c r="B159" s="85"/>
+      <c r="B159" s="95"/>
       <c r="C159" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D159" s="21" t="s">
         <v>173</v>
@@ -7696,24 +7659,24 @@
         <v>173</v>
       </c>
       <c r="F159" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="G159" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="G159" s="21" t="s">
+      <c r="H159" s="11" t="s">
         <v>200</v>
-      </c>
-      <c r="H159" s="11" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="160" spans="1:8">
       <c r="A160" s="19">
         <v>14</v>
       </c>
-      <c r="B160" s="86" t="s">
+      <c r="B160" s="90" t="s">
         <v>8</v>
       </c>
       <c r="C160" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D160" s="21" t="s">
         <v>173</v>
@@ -7722,22 +7685,22 @@
         <v>173</v>
       </c>
       <c r="F160" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G160" s="21" t="s">
         <v>175</v>
       </c>
       <c r="H160" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="161" spans="1:8">
       <c r="A161" s="19">
         <v>15</v>
       </c>
-      <c r="B161" s="83"/>
+      <c r="B161" s="91"/>
       <c r="C161" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D161" s="21" t="s">
         <v>173</v>
@@ -7746,24 +7709,24 @@
         <v>173</v>
       </c>
       <c r="F161" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G161" s="21" t="s">
         <v>175</v>
       </c>
       <c r="H161" s="11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="162" spans="1:8">
       <c r="A162" s="70">
         <v>16</v>
       </c>
-      <c r="B162" s="77" t="s">
+      <c r="B162" s="108" t="s">
         <v>9</v>
       </c>
       <c r="C162" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D162" s="21" t="s">
         <v>173</v>
@@ -7772,7 +7735,7 @@
         <v>173</v>
       </c>
       <c r="F162" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G162" s="69" t="s">
         <v>175</v>
@@ -7783,9 +7746,9 @@
       <c r="A163" s="70">
         <v>17</v>
       </c>
-      <c r="B163" s="87"/>
+      <c r="B163" s="110"/>
       <c r="C163" s="69" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D163" s="68" t="s">
         <v>173</v>
@@ -7798,16 +7761,16 @@
         <v>175</v>
       </c>
       <c r="H163" s="72" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="164" spans="1:8">
       <c r="A164" s="70">
         <v>18</v>
       </c>
-      <c r="B164" s="85"/>
+      <c r="B164" s="95"/>
       <c r="C164" s="65" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D164" s="21" t="s">
         <v>173</v>
@@ -7817,7 +7780,7 @@
       </c>
       <c r="F164" s="21"/>
       <c r="G164" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="H164" s="11"/>
     </row>
@@ -7825,11 +7788,11 @@
       <c r="A165" s="70">
         <v>19</v>
       </c>
-      <c r="B165" s="86" t="s">
+      <c r="B165" s="90" t="s">
         <v>11</v>
       </c>
       <c r="C165" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D165" s="21" t="s">
         <v>173</v>
@@ -7838,10 +7801,10 @@
         <v>173</v>
       </c>
       <c r="F165" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="G165" s="21" t="s">
         <v>212</v>
-      </c>
-      <c r="G165" s="21" t="s">
-        <v>213</v>
       </c>
       <c r="H165" s="11"/>
     </row>
@@ -7849,9 +7812,9 @@
       <c r="A166" s="70">
         <v>20</v>
       </c>
-      <c r="B166" s="83"/>
+      <c r="B166" s="91"/>
       <c r="C166" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D166" s="21" t="s">
         <v>173</v>
@@ -7861,7 +7824,7 @@
       </c>
       <c r="F166" s="21"/>
       <c r="G166" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H166" s="11"/>
     </row>
@@ -7869,9 +7832,9 @@
       <c r="A167" s="70">
         <v>21</v>
       </c>
-      <c r="B167" s="83"/>
+      <c r="B167" s="91"/>
       <c r="C167" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D167" s="21" t="s">
         <v>173</v>
@@ -7881,7 +7844,7 @@
       </c>
       <c r="F167" s="21"/>
       <c r="G167" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H167" s="11"/>
     </row>
@@ -7889,9 +7852,9 @@
       <c r="A168" s="70">
         <v>22</v>
       </c>
-      <c r="B168" s="83"/>
+      <c r="B168" s="91"/>
       <c r="C168" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D168" s="21" t="s">
         <v>173</v>
@@ -7901,7 +7864,7 @@
       </c>
       <c r="F168" s="21"/>
       <c r="G168" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H168" s="11"/>
     </row>
@@ -7909,9 +7872,9 @@
       <c r="A169" s="70">
         <v>23</v>
       </c>
-      <c r="B169" s="83"/>
+      <c r="B169" s="91"/>
       <c r="C169" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D169" s="21" t="s">
         <v>173</v>
@@ -7921,7 +7884,7 @@
       </c>
       <c r="F169" s="21"/>
       <c r="G169" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H169" s="11"/>
     </row>
@@ -7929,9 +7892,9 @@
       <c r="A170" s="70">
         <v>24</v>
       </c>
-      <c r="B170" s="83"/>
+      <c r="B170" s="91"/>
       <c r="C170" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D170" s="21" t="s">
         <v>173</v>
@@ -7941,7 +7904,7 @@
       </c>
       <c r="F170" s="21"/>
       <c r="G170" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H170" s="11"/>
     </row>
@@ -7949,9 +7912,9 @@
       <c r="A171" s="70">
         <v>25</v>
       </c>
-      <c r="B171" s="83"/>
+      <c r="B171" s="91"/>
       <c r="C171" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D171" s="21" t="s">
         <v>173</v>
@@ -7961,7 +7924,7 @@
       </c>
       <c r="F171" s="21"/>
       <c r="G171" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H171" s="11"/>
     </row>
@@ -7969,7 +7932,7 @@
       <c r="A172" s="70">
         <v>26</v>
       </c>
-      <c r="B172" s="83"/>
+      <c r="B172" s="91"/>
       <c r="C172" s="21" t="s">
         <v>51</v>
       </c>
@@ -7981,7 +7944,7 @@
       </c>
       <c r="F172" s="21"/>
       <c r="G172" s="21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H172" s="11"/>
     </row>
@@ -7989,11 +7952,11 @@
       <c r="A173" s="19">
         <v>27</v>
       </c>
-      <c r="B173" s="86" t="s">
+      <c r="B173" s="90" t="s">
         <v>13</v>
       </c>
       <c r="C173" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D173" s="21" t="s">
         <v>173</v>
@@ -8002,10 +7965,10 @@
         <v>173</v>
       </c>
       <c r="F173" s="71" t="s">
+        <v>220</v>
+      </c>
+      <c r="G173" s="22" t="s">
         <v>221</v>
-      </c>
-      <c r="G173" s="22" t="s">
-        <v>222</v>
       </c>
       <c r="H173" s="11"/>
     </row>
@@ -8013,9 +7976,9 @@
       <c r="A174" s="19">
         <v>28</v>
       </c>
-      <c r="B174" s="83"/>
+      <c r="B174" s="91"/>
       <c r="C174" s="65" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D174" s="21" t="s">
         <v>173</v>
@@ -8024,10 +7987,10 @@
         <v>173</v>
       </c>
       <c r="F174" s="65" t="s">
+        <v>223</v>
+      </c>
+      <c r="G174" s="65" t="s">
         <v>224</v>
-      </c>
-      <c r="G174" s="65" t="s">
-        <v>225</v>
       </c>
       <c r="H174" s="11"/>
     </row>
@@ -8035,9 +7998,9 @@
       <c r="A175" s="19">
         <v>29</v>
       </c>
-      <c r="B175" s="83"/>
+      <c r="B175" s="91"/>
       <c r="C175" s="21" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D175" s="21" t="s">
         <v>173</v>
@@ -8046,10 +8009,10 @@
         <v>173</v>
       </c>
       <c r="F175" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="G175" s="21" t="s">
         <v>227</v>
-      </c>
-      <c r="G175" s="21" t="s">
-        <v>228</v>
       </c>
       <c r="H175" s="11"/>
     </row>
@@ -8057,11 +8020,11 @@
       <c r="A176" s="19">
         <v>30</v>
       </c>
-      <c r="B176" s="77" t="s">
+      <c r="B176" s="108" t="s">
         <v>14</v>
       </c>
       <c r="C176" s="21" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D176" s="21" t="s">
         <v>173</v>
@@ -8070,22 +8033,22 @@
         <v>173</v>
       </c>
       <c r="F176" s="21" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G176" s="21" t="s">
         <v>175</v>
       </c>
       <c r="H176" s="11" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="177" spans="1:8">
       <c r="A177" s="23">
         <v>31</v>
       </c>
-      <c r="B177" s="78"/>
+      <c r="B177" s="109"/>
       <c r="C177" s="20" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D177" s="20" t="s">
         <v>173</v>
@@ -8094,24 +8057,24 @@
         <v>173</v>
       </c>
       <c r="F177" s="20" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G177" s="20" t="s">
         <v>175</v>
       </c>
       <c r="H177" s="24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="178" spans="1:8">
       <c r="A178" s="16">
         <v>32</v>
       </c>
-      <c r="B178" s="79" t="s">
+      <c r="B178" s="111" t="s">
+        <v>233</v>
+      </c>
+      <c r="C178" s="66" t="s">
         <v>234</v>
-      </c>
-      <c r="C178" s="66" t="s">
-        <v>235</v>
       </c>
       <c r="D178" s="17" t="s">
         <v>173</v>
@@ -8120,10 +8083,10 @@
         <v>173</v>
       </c>
       <c r="F178" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="G178" s="66" t="s">
         <v>236</v>
-      </c>
-      <c r="G178" s="66" t="s">
-        <v>237</v>
       </c>
       <c r="H178" s="10"/>
     </row>
@@ -8131,9 +8094,9 @@
       <c r="A179" s="19">
         <v>33</v>
       </c>
-      <c r="B179" s="80"/>
+      <c r="B179" s="112"/>
       <c r="C179" s="65" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D179" s="21" t="s">
         <v>173</v>
@@ -8142,10 +8105,10 @@
         <v>173</v>
       </c>
       <c r="F179" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="G179" s="67" t="s">
         <v>239</v>
-      </c>
-      <c r="G179" s="67" t="s">
-        <v>240</v>
       </c>
       <c r="H179" s="11"/>
     </row>
@@ -8153,9 +8116,9 @@
       <c r="A180" s="19">
         <v>34</v>
       </c>
-      <c r="B180" s="81"/>
+      <c r="B180" s="113"/>
       <c r="C180" s="67" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D180" s="21" t="s">
         <v>173</v>
@@ -8164,10 +8127,10 @@
         <v>173</v>
       </c>
       <c r="F180" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="G180" s="20" t="s">
         <v>239</v>
-      </c>
-      <c r="G180" s="20" t="s">
-        <v>240</v>
       </c>
       <c r="H180" s="24"/>
     </row>
@@ -8175,9 +8138,9 @@
       <c r="A181" s="25">
         <v>35</v>
       </c>
-      <c r="B181" s="81"/>
+      <c r="B181" s="113"/>
       <c r="C181" s="67" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D181" s="26" t="s">
         <v>173</v>
@@ -8186,10 +8149,10 @@
         <v>173</v>
       </c>
       <c r="F181" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="G181" s="67" t="s">
         <v>243</v>
-      </c>
-      <c r="G181" s="67" t="s">
-        <v>244</v>
       </c>
       <c r="H181" s="27"/>
     </row>
@@ -8197,9 +8160,9 @@
       <c r="A182" s="28">
         <v>36</v>
       </c>
-      <c r="B182" s="82"/>
+      <c r="B182" s="99"/>
       <c r="C182" s="29" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D182" s="29" t="s">
         <v>173</v>
@@ -8213,314 +8176,314 @@
     </row>
     <row r="183" spans="1:8">
       <c r="A183" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B183" s="1" t="s">
         <v>246</v>
-      </c>
-      <c r="B183" s="1" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="184" spans="1:8">
       <c r="B184" s="31" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="185" spans="1:8">
       <c r="B185" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="195" spans="1:7">
       <c r="A195" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B195" s="1" t="s">
         <v>250</v>
-      </c>
-      <c r="B195" s="1" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="196" spans="1:7">
       <c r="A196" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B196" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="B196" s="32" t="s">
+      <c r="C196" s="81" t="s">
         <v>253</v>
       </c>
-      <c r="C196" s="109" t="s">
+      <c r="D196" s="81"/>
+      <c r="E196" s="81"/>
+      <c r="F196" s="33" t="s">
         <v>254</v>
       </c>
-      <c r="D196" s="109"/>
-      <c r="E196" s="109"/>
-      <c r="F196" s="33" t="s">
+      <c r="G196" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="G196" s="34" t="s">
+    </row>
+    <row r="197" spans="1:7">
+      <c r="A197" s="106" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="197" spans="1:7">
-      <c r="A197" s="92" t="s">
+      <c r="B197" s="91" t="s">
         <v>257</v>
       </c>
-      <c r="B197" s="83" t="s">
+      <c r="C197" s="82" t="s">
         <v>258</v>
       </c>
-      <c r="C197" s="110" t="s">
+      <c r="D197" s="83"/>
+      <c r="E197" s="83"/>
+      <c r="F197" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="D197" s="111"/>
-      <c r="E197" s="111"/>
-      <c r="F197" s="21" t="s">
+      <c r="G197" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="G197" s="35" t="s">
+    </row>
+    <row r="198" spans="1:7">
+      <c r="A198" s="106"/>
+      <c r="B198" s="114"/>
+      <c r="C198" s="84" t="s">
+        <v>258</v>
+      </c>
+      <c r="D198" s="85"/>
+      <c r="E198" s="85"/>
+      <c r="F198" s="20" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="198" spans="1:7">
-      <c r="A198" s="92"/>
-      <c r="B198" s="84"/>
-      <c r="C198" s="102" t="s">
+      <c r="G198" s="36" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7">
+      <c r="A199" s="106"/>
+      <c r="B199" s="91" t="s">
+        <v>262</v>
+      </c>
+      <c r="C199" s="86" t="s">
+        <v>263</v>
+      </c>
+      <c r="D199" s="86"/>
+      <c r="E199" s="86"/>
+      <c r="F199" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="D198" s="112"/>
-      <c r="E198" s="112"/>
-      <c r="F198" s="20" t="s">
-        <v>262</v>
-      </c>
-      <c r="G198" s="36" t="s">
+      <c r="G199" s="35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7">
+      <c r="A200" s="106"/>
+      <c r="B200" s="91"/>
+      <c r="C200" s="84" t="s">
+        <v>263</v>
+      </c>
+      <c r="D200" s="84"/>
+      <c r="E200" s="84"/>
+      <c r="F200" s="21" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="199" spans="1:7">
-      <c r="A199" s="92"/>
-      <c r="B199" s="83" t="s">
-        <v>263</v>
-      </c>
-      <c r="C199" s="113" t="s">
+      <c r="G200" s="35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7">
+      <c r="A201" s="106"/>
+      <c r="B201" s="114" t="s">
         <v>264</v>
       </c>
-      <c r="D199" s="113"/>
-      <c r="E199" s="113"/>
-      <c r="F199" s="21" t="s">
+      <c r="C201" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D201" s="88"/>
+      <c r="E201" s="89"/>
+      <c r="F201" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="G201" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="G199" s="35" t="s">
+    </row>
+    <row r="202" spans="1:7">
+      <c r="A202" s="106"/>
+      <c r="B202" s="95"/>
+      <c r="C202" s="87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D202" s="88"/>
+      <c r="E202" s="89"/>
+      <c r="F202" s="21" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="200" spans="1:7">
-      <c r="A200" s="92"/>
-      <c r="B200" s="83"/>
-      <c r="C200" s="102" t="s">
-        <v>264</v>
-      </c>
-      <c r="D200" s="102"/>
-      <c r="E200" s="102"/>
-      <c r="F200" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="G200" s="35" t="s">
+      <c r="G202" s="35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7">
+      <c r="A203" s="106"/>
+      <c r="B203" s="91" t="s">
+        <v>265</v>
+      </c>
+      <c r="C203" s="86" t="s">
+        <v>266</v>
+      </c>
+      <c r="D203" s="86"/>
+      <c r="E203" s="86"/>
+      <c r="F203" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="G203" s="35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7">
+      <c r="A204" s="106"/>
+      <c r="B204" s="91"/>
+      <c r="C204" s="86" t="s">
+        <v>266</v>
+      </c>
+      <c r="D204" s="86"/>
+      <c r="E204" s="86"/>
+      <c r="F204" s="21" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="201" spans="1:7">
-      <c r="A201" s="92"/>
-      <c r="B201" s="84" t="s">
-        <v>265</v>
-      </c>
-      <c r="C201" s="103" t="s">
+      <c r="G204" s="35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="205" spans="1:7">
+      <c r="A205" s="106" t="s">
+        <v>267</v>
+      </c>
+      <c r="B205" s="91" t="s">
+        <v>268</v>
+      </c>
+      <c r="C205" s="90" t="s">
+        <v>269</v>
+      </c>
+      <c r="D205" s="91"/>
+      <c r="E205" s="91"/>
+      <c r="F205" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="D201" s="104"/>
-      <c r="E201" s="105"/>
-      <c r="F201" s="21" t="s">
+      <c r="G205" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="G201" s="35" t="s">
+    </row>
+    <row r="206" spans="1:7">
+      <c r="A206" s="106"/>
+      <c r="B206" s="91"/>
+      <c r="C206" s="91" t="s">
+        <v>270</v>
+      </c>
+      <c r="D206" s="91"/>
+      <c r="E206" s="91"/>
+      <c r="F206" s="21" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="202" spans="1:7">
-      <c r="A202" s="92"/>
-      <c r="B202" s="85"/>
-      <c r="C202" s="103" t="s">
+      <c r="G206" s="35" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7">
+      <c r="A207" s="106"/>
+      <c r="B207" s="91" t="s">
+        <v>272</v>
+      </c>
+      <c r="C207" s="91" t="s">
+        <v>273</v>
+      </c>
+      <c r="D207" s="91"/>
+      <c r="E207" s="91"/>
+      <c r="F207" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="D202" s="104"/>
-      <c r="E202" s="105"/>
-      <c r="F202" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="G202" s="35" t="s">
+      <c r="G207" s="35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7">
+      <c r="A208" s="106"/>
+      <c r="B208" s="91"/>
+      <c r="C208" s="91" t="s">
+        <v>274</v>
+      </c>
+      <c r="D208" s="91"/>
+      <c r="E208" s="91"/>
+      <c r="F208" s="21" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="203" spans="1:7">
-      <c r="A203" s="92"/>
-      <c r="B203" s="83" t="s">
-        <v>266</v>
-      </c>
-      <c r="C203" s="102" t="s">
-        <v>267</v>
-      </c>
-      <c r="D203" s="102"/>
-      <c r="E203" s="102"/>
-      <c r="F203" s="21" t="s">
+      <c r="G208" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="G203" s="35" t="s">
+    </row>
+    <row r="209" spans="1:7">
+      <c r="A209" s="106" t="s">
+        <v>275</v>
+      </c>
+      <c r="B209" s="91" t="s">
+        <v>276</v>
+      </c>
+      <c r="C209" s="90" t="s">
+        <v>277</v>
+      </c>
+      <c r="D209" s="91"/>
+      <c r="E209" s="91"/>
+      <c r="F209" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="G209" s="35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7">
+      <c r="A210" s="106"/>
+      <c r="B210" s="91"/>
+      <c r="C210" s="91" t="s">
+        <v>278</v>
+      </c>
+      <c r="D210" s="91"/>
+      <c r="E210" s="91"/>
+      <c r="F210" s="21" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="204" spans="1:7">
-      <c r="A204" s="92"/>
-      <c r="B204" s="83"/>
-      <c r="C204" s="102" t="s">
-        <v>267</v>
-      </c>
-      <c r="D204" s="102"/>
-      <c r="E204" s="102"/>
-      <c r="F204" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="G204" s="35" t="s">
+      <c r="G210" s="35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7">
+      <c r="A211" s="106"/>
+      <c r="B211" s="91" t="s">
+        <v>279</v>
+      </c>
+      <c r="C211" s="90" t="s">
+        <v>280</v>
+      </c>
+      <c r="D211" s="91"/>
+      <c r="E211" s="91"/>
+      <c r="F211" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="G211" s="35" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7">
+      <c r="A212" s="107"/>
+      <c r="B212" s="92"/>
+      <c r="C212" s="92" t="s">
+        <v>281</v>
+      </c>
+      <c r="D212" s="92"/>
+      <c r="E212" s="92"/>
+      <c r="F212" s="29" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="205" spans="1:7">
-      <c r="A205" s="92" t="s">
-        <v>268</v>
-      </c>
-      <c r="B205" s="83" t="s">
-        <v>269</v>
-      </c>
-      <c r="C205" s="86" t="s">
-        <v>270</v>
-      </c>
-      <c r="D205" s="83"/>
-      <c r="E205" s="83"/>
-      <c r="F205" s="21" t="s">
+      <c r="G212" s="37" t="s">
         <v>260</v>
-      </c>
-      <c r="G205" s="35" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="206" spans="1:7">
-      <c r="A206" s="92"/>
-      <c r="B206" s="83"/>
-      <c r="C206" s="83" t="s">
-        <v>271</v>
-      </c>
-      <c r="D206" s="83"/>
-      <c r="E206" s="83"/>
-      <c r="F206" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="G206" s="35" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="207" spans="1:7">
-      <c r="A207" s="92"/>
-      <c r="B207" s="83" t="s">
-        <v>273</v>
-      </c>
-      <c r="C207" s="83" t="s">
-        <v>274</v>
-      </c>
-      <c r="D207" s="83"/>
-      <c r="E207" s="83"/>
-      <c r="F207" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="G207" s="35" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="208" spans="1:7">
-      <c r="A208" s="92"/>
-      <c r="B208" s="83"/>
-      <c r="C208" s="83" t="s">
-        <v>275</v>
-      </c>
-      <c r="D208" s="83"/>
-      <c r="E208" s="83"/>
-      <c r="F208" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="G208" s="35" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="209" spans="1:7">
-      <c r="A209" s="92" t="s">
-        <v>276</v>
-      </c>
-      <c r="B209" s="83" t="s">
-        <v>277</v>
-      </c>
-      <c r="C209" s="86" t="s">
-        <v>278</v>
-      </c>
-      <c r="D209" s="83"/>
-      <c r="E209" s="83"/>
-      <c r="F209" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="G209" s="35" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="210" spans="1:7">
-      <c r="A210" s="92"/>
-      <c r="B210" s="83"/>
-      <c r="C210" s="83" t="s">
-        <v>279</v>
-      </c>
-      <c r="D210" s="83"/>
-      <c r="E210" s="83"/>
-      <c r="F210" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="G210" s="35" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="211" spans="1:7">
-      <c r="A211" s="92"/>
-      <c r="B211" s="83" t="s">
-        <v>280</v>
-      </c>
-      <c r="C211" s="86" t="s">
-        <v>281</v>
-      </c>
-      <c r="D211" s="83"/>
-      <c r="E211" s="83"/>
-      <c r="F211" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="G211" s="35" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="212" spans="1:7">
-      <c r="A212" s="93"/>
-      <c r="B212" s="94"/>
-      <c r="C212" s="94" t="s">
-        <v>282</v>
-      </c>
-      <c r="D212" s="94"/>
-      <c r="E212" s="94"/>
-      <c r="F212" s="29" t="s">
-        <v>262</v>
-      </c>
-      <c r="G212" s="37" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="213" spans="1:7">
       <c r="A213" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C213" s="31"/>
       <c r="D213" s="31"/>
@@ -8539,7 +8502,7 @@
     </row>
     <row r="216" spans="1:7">
       <c r="A216" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C216" s="31"/>
       <c r="D216" s="31"/>
@@ -8547,87 +8510,87 @@
     </row>
     <row r="217" spans="1:7">
       <c r="A217" s="38" t="s">
+        <v>284</v>
+      </c>
+      <c r="B217" s="93" t="s">
         <v>285</v>
       </c>
-      <c r="B217" s="100" t="s">
+      <c r="C217" s="93"/>
+      <c r="D217" s="93"/>
+      <c r="E217" s="93"/>
+      <c r="F217" s="39" t="s">
         <v>286</v>
       </c>
-      <c r="C217" s="100"/>
-      <c r="D217" s="100"/>
-      <c r="E217" s="100"/>
-      <c r="F217" s="39" t="s">
+      <c r="G217" s="40" t="s">
         <v>287</v>
-      </c>
-      <c r="G217" s="40" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="218" spans="1:7" ht="93" customHeight="1">
       <c r="A218" s="41" t="s">
+        <v>288</v>
+      </c>
+      <c r="B218" s="94" t="s">
         <v>289</v>
       </c>
-      <c r="B218" s="101" t="s">
-        <v>290</v>
-      </c>
-      <c r="C218" s="85"/>
-      <c r="D218" s="85"/>
-      <c r="E218" s="85"/>
+      <c r="C218" s="95"/>
+      <c r="D218" s="95"/>
+      <c r="E218" s="95"/>
       <c r="F218" s="42" t="s">
         <v>158</v>
       </c>
       <c r="G218" s="43" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="219" spans="1:7" ht="57" customHeight="1">
       <c r="A219" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="B219" s="96" t="s">
         <v>291</v>
-      </c>
-      <c r="B219" s="96" t="s">
-        <v>292</v>
       </c>
       <c r="C219" s="97"/>
       <c r="D219" s="97"/>
       <c r="E219" s="98"/>
       <c r="F219" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G219" s="11" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="220" spans="1:7" ht="57" customHeight="1">
       <c r="A220" s="12" t="s">
+        <v>292</v>
+      </c>
+      <c r="B220" s="96" t="s">
         <v>293</v>
-      </c>
-      <c r="B220" s="96" t="s">
-        <v>294</v>
       </c>
       <c r="C220" s="97"/>
       <c r="D220" s="97"/>
       <c r="E220" s="98"/>
       <c r="F220" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G220" s="24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="221" spans="1:7" ht="69" customHeight="1">
       <c r="A221" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="B221" s="99" t="s">
         <v>295</v>
       </c>
-      <c r="B221" s="82" t="s">
-        <v>296</v>
-      </c>
-      <c r="C221" s="94"/>
-      <c r="D221" s="94"/>
-      <c r="E221" s="94"/>
+      <c r="C221" s="92"/>
+      <c r="D221" s="92"/>
+      <c r="E221" s="92"/>
       <c r="F221" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G221" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="222" spans="1:7">
@@ -8635,26 +8598,26 @@
     </row>
     <row r="224" spans="1:7">
       <c r="A224" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="225" spans="1:7">
       <c r="A225" s="4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B225" s="32" t="s">
         <v>137</v>
       </c>
       <c r="C225" s="45" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D225" s="46" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E225" s="46"/>
       <c r="F225" s="47"/>
       <c r="G225" s="34" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="226" spans="1:7">
@@ -8665,13 +8628,13 @@
         <v>1.04</v>
       </c>
       <c r="C226" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="D226" s="100" t="s">
         <v>301</v>
       </c>
-      <c r="D226" s="99" t="s">
-        <v>302</v>
-      </c>
-      <c r="E226" s="99"/>
-      <c r="F226" s="99"/>
+      <c r="E226" s="100"/>
+      <c r="F226" s="100"/>
       <c r="G226" s="50"/>
     </row>
     <row r="227" spans="1:7">
@@ -8682,13 +8645,13 @@
         <v>1.05</v>
       </c>
       <c r="C227" s="21" t="s">
-        <v>301</v>
-      </c>
-      <c r="D227" s="95" t="s">
-        <v>303</v>
-      </c>
-      <c r="E227" s="95"/>
-      <c r="F227" s="95"/>
+        <v>300</v>
+      </c>
+      <c r="D227" s="101" t="s">
+        <v>302</v>
+      </c>
+      <c r="E227" s="101"/>
+      <c r="F227" s="101"/>
       <c r="G227" s="35"/>
     </row>
     <row r="228" spans="1:7">
@@ -8699,13 +8662,13 @@
         <v>1.06</v>
       </c>
       <c r="C228" s="21" t="s">
-        <v>301</v>
-      </c>
-      <c r="D228" s="95" t="s">
-        <v>304</v>
-      </c>
-      <c r="E228" s="95"/>
-      <c r="F228" s="95"/>
+        <v>300</v>
+      </c>
+      <c r="D228" s="101" t="s">
+        <v>303</v>
+      </c>
+      <c r="E228" s="101"/>
+      <c r="F228" s="101"/>
       <c r="G228" s="35"/>
     </row>
     <row r="229" spans="1:7">
@@ -8716,13 +8679,13 @@
         <v>1.07</v>
       </c>
       <c r="C229" s="21" t="s">
-        <v>301</v>
-      </c>
-      <c r="D229" s="95" t="s">
-        <v>305</v>
-      </c>
-      <c r="E229" s="95"/>
-      <c r="F229" s="95"/>
+        <v>300</v>
+      </c>
+      <c r="D229" s="101" t="s">
+        <v>304</v>
+      </c>
+      <c r="E229" s="101"/>
+      <c r="F229" s="101"/>
       <c r="G229" s="35"/>
     </row>
     <row r="230" spans="1:7">
@@ -8733,13 +8696,13 @@
         <v>1.08</v>
       </c>
       <c r="C230" s="21" t="s">
-        <v>301</v>
-      </c>
-      <c r="D230" s="95" t="s">
-        <v>306</v>
-      </c>
-      <c r="E230" s="95"/>
-      <c r="F230" s="95"/>
+        <v>300</v>
+      </c>
+      <c r="D230" s="101" t="s">
+        <v>305</v>
+      </c>
+      <c r="E230" s="101"/>
+      <c r="F230" s="101"/>
       <c r="G230" s="35"/>
     </row>
     <row r="231" spans="1:7">
@@ -8750,13 +8713,13 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="C231" s="21" t="s">
-        <v>301</v>
-      </c>
-      <c r="D231" s="95" t="s">
-        <v>307</v>
-      </c>
-      <c r="E231" s="95"/>
-      <c r="F231" s="95"/>
+        <v>300</v>
+      </c>
+      <c r="D231" s="101" t="s">
+        <v>306</v>
+      </c>
+      <c r="E231" s="101"/>
+      <c r="F231" s="101"/>
       <c r="G231" s="35"/>
     </row>
     <row r="232" spans="1:7">
@@ -8767,13 +8730,13 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C232" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="D232" s="88" t="s">
-        <v>308</v>
-      </c>
-      <c r="E232" s="89"/>
-      <c r="F232" s="90"/>
+        <v>300</v>
+      </c>
+      <c r="D232" s="102" t="s">
+        <v>307</v>
+      </c>
+      <c r="E232" s="103"/>
+      <c r="F232" s="104"/>
       <c r="G232" s="36"/>
     </row>
     <row r="233" spans="1:7">
@@ -8784,13 +8747,13 @@
         <v>1.1100000000000001</v>
       </c>
       <c r="C233" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="D233" s="88" t="s">
-        <v>309</v>
-      </c>
-      <c r="E233" s="89"/>
-      <c r="F233" s="90"/>
+        <v>300</v>
+      </c>
+      <c r="D233" s="102" t="s">
+        <v>308</v>
+      </c>
+      <c r="E233" s="103"/>
+      <c r="F233" s="104"/>
       <c r="G233" s="36"/>
     </row>
     <row r="234" spans="1:7">
@@ -8801,13 +8764,13 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="C234" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="D234" s="88" t="s">
-        <v>310</v>
-      </c>
-      <c r="E234" s="89"/>
-      <c r="F234" s="90"/>
+        <v>300</v>
+      </c>
+      <c r="D234" s="102" t="s">
+        <v>309</v>
+      </c>
+      <c r="E234" s="103"/>
+      <c r="F234" s="104"/>
       <c r="G234" s="36"/>
     </row>
     <row r="235" spans="1:7">
@@ -8818,10 +8781,10 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="C235" s="20" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D235" s="55" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E235" s="56"/>
       <c r="F235" s="57"/>
@@ -8835,10 +8798,10 @@
         <v>1.1399999999999999</v>
       </c>
       <c r="C236" s="20" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D236" s="55" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E236" s="56"/>
       <c r="F236" s="57"/>
@@ -8852,10 +8815,10 @@
         <v>1.1499999999999999</v>
       </c>
       <c r="C237" s="20" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D237" s="55" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E237" s="56"/>
       <c r="F237" s="57"/>
@@ -8869,17 +8832,17 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="C238" s="29" t="s">
-        <v>301</v>
-      </c>
-      <c r="D238" s="91" t="s">
-        <v>314</v>
-      </c>
-      <c r="E238" s="91"/>
-      <c r="F238" s="91"/>
+        <v>300</v>
+      </c>
+      <c r="D238" s="105" t="s">
+        <v>313</v>
+      </c>
+      <c r="E238" s="105"/>
+      <c r="F238" s="105"/>
       <c r="G238" s="37"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="gtdd3/U9jncnsyB36nF4pUNeFQ9YgVOqxdH24Q2fl98kFdxWe2F6JcdX958pldXuL/TiX03wmHo1bSzDZyBHGQ==" saltValue="A3+sq91Jqztcpa19NEUyIQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="0UT41XaxqgQhfsgssrlya0NBWnXPg0uj6FDdbXVfzp9AG3o5yGtUIGPEnJmecspgIgyYg7bYBIYw+0kw8uPBjA==" saltValue="4z6ntY5HlVVddlUdMd47dg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <customSheetViews>
     <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}" scale="115" topLeftCell="A157">
       <selection activeCell="F172" sqref="F172"/>
@@ -8888,31 +8851,16 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="51">
-    <mergeCell ref="F111:N111"/>
-    <mergeCell ref="C196:E196"/>
-    <mergeCell ref="C197:E197"/>
-    <mergeCell ref="C198:E198"/>
-    <mergeCell ref="C199:E199"/>
-    <mergeCell ref="C200:E200"/>
-    <mergeCell ref="C201:E201"/>
-    <mergeCell ref="C202:E202"/>
-    <mergeCell ref="C203:E203"/>
-    <mergeCell ref="C204:E204"/>
-    <mergeCell ref="C205:E205"/>
-    <mergeCell ref="C206:E206"/>
-    <mergeCell ref="C207:E207"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="B217:E217"/>
-    <mergeCell ref="B218:E218"/>
-    <mergeCell ref="B219:E219"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:E221"/>
-    <mergeCell ref="D226:F226"/>
-    <mergeCell ref="D227:F227"/>
+    <mergeCell ref="B176:B177"/>
+    <mergeCell ref="B178:B182"/>
+    <mergeCell ref="B197:B198"/>
+    <mergeCell ref="B199:B200"/>
+    <mergeCell ref="B201:B202"/>
+    <mergeCell ref="B147:B159"/>
+    <mergeCell ref="B160:B161"/>
+    <mergeCell ref="B162:B164"/>
+    <mergeCell ref="B165:B172"/>
+    <mergeCell ref="B173:B175"/>
     <mergeCell ref="D233:F233"/>
     <mergeCell ref="D234:F234"/>
     <mergeCell ref="D238:F238"/>
@@ -8929,16 +8877,31 @@
     <mergeCell ref="D230:F230"/>
     <mergeCell ref="D231:F231"/>
     <mergeCell ref="D232:F232"/>
-    <mergeCell ref="B147:B159"/>
-    <mergeCell ref="B160:B161"/>
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="B165:B172"/>
-    <mergeCell ref="B173:B175"/>
-    <mergeCell ref="B176:B177"/>
-    <mergeCell ref="B178:B182"/>
-    <mergeCell ref="B197:B198"/>
-    <mergeCell ref="B199:B200"/>
-    <mergeCell ref="B201:B202"/>
+    <mergeCell ref="B219:E219"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:E221"/>
+    <mergeCell ref="D226:F226"/>
+    <mergeCell ref="D227:F227"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="B217:E217"/>
+    <mergeCell ref="B218:E218"/>
+    <mergeCell ref="C205:E205"/>
+    <mergeCell ref="C206:E206"/>
+    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C200:E200"/>
+    <mergeCell ref="C201:E201"/>
+    <mergeCell ref="C202:E202"/>
+    <mergeCell ref="C203:E203"/>
+    <mergeCell ref="C204:E204"/>
+    <mergeCell ref="F111:N111"/>
+    <mergeCell ref="C196:E196"/>
+    <mergeCell ref="C197:E197"/>
+    <mergeCell ref="C198:E198"/>
+    <mergeCell ref="C199:E199"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -8956,20 +8919,20 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
+    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
+      <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{16B2C8B3-13FA-43FB-96C1-3763C72619A6}">
       <selection activeCell="E26" sqref="E26"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{179F0E1F-F6F7-410E-B883-54B8A90BA550}">
-      <selection activeCell="E26" sqref="E26"/>
+    <customSheetView guid="{E811CF45-D5B3-4449-84AE-1514F9E9258F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>